<commit_message>
improve source code with basler camera
</commit_message>
<xml_diff>
--- a/ObjectDetection/Automatic Product Counting Machine/testExcel/test.xlsx
+++ b/ObjectDetection/Automatic Product Counting Machine/testExcel/test.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A391652-0284-45C7-9FB9-4BE356F1EED9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" firstSheet="11" activeTab="15"/>
+    <workbookView xWindow="615" yWindow="735" windowWidth="7935" windowHeight="11295" firstSheet="15" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,6 +24,7 @@
     <sheet name="Sheet14" sheetId="14" r:id="rId14"/>
     <sheet name="Sheet15" sheetId="15" r:id="rId15"/>
     <sheet name="Sheet16" sheetId="16" r:id="rId16"/>
+    <sheet name="Sheet17" sheetId="17" r:id="rId17"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
@@ -40,7 +42,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -165,6 +167,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -200,6 +219,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -375,16 +411,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>31</v>
       </c>
@@ -392,7 +428,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
         <v>0</v>
       </c>
@@ -400,7 +436,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>31</v>
       </c>
@@ -408,7 +444,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
         <v>1</v>
       </c>
@@ -416,12 +452,12 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>31</v>
       </c>
@@ -432,16 +468,16 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>37</v>
       </c>
@@ -449,7 +485,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>73</v>
       </c>
@@ -478,12 +514,12 @@
         <v>206</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C3">
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>73</v>
       </c>
@@ -503,17 +539,17 @@
         <v>174</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>95</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C6">
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E7">
         <v>31</v>
       </c>
@@ -536,7 +572,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E10">
         <v>29</v>
       </c>
@@ -547,7 +583,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E13">
         <v>32</v>
       </c>
@@ -573,16 +609,16 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="B3:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>221</v>
       </c>
@@ -590,27 +626,27 @@
         <v>235</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I4">
         <v>252</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="F5">
         <v>132</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D8">
         <v>221</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C11">
         <v>96</v>
       </c>
@@ -621,16 +657,16 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="C4:M13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="4" spans="3:13" x14ac:dyDescent="0.3">
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="4" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C4">
         <v>28</v>
       </c>
@@ -653,12 +689,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="8" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:13" x14ac:dyDescent="0.25">
       <c r="H8">
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="3:13" x14ac:dyDescent="0.25">
       <c r="M13">
         <v>31</v>
       </c>
@@ -669,16 +705,16 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A3:K19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C3">
         <v>267</v>
       </c>
@@ -692,7 +728,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>54</v>
       </c>
@@ -706,7 +742,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G9">
         <v>37</v>
       </c>
@@ -714,27 +750,27 @@
         <v>72</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K10">
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K13">
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H14">
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C18">
         <v>54</v>
       </c>
@@ -742,7 +778,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:9" x14ac:dyDescent="0.25">
       <c r="E19">
         <v>36</v>
       </c>
@@ -753,21 +789,21 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="B1:J23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="2:9" x14ac:dyDescent="0.3">
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B1">
         <v>96</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C4">
         <v>90</v>
       </c>
@@ -778,7 +814,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C7">
         <v>0</v>
       </c>
@@ -792,7 +828,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C10">
         <v>36</v>
       </c>
@@ -800,7 +836,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D14">
         <v>36</v>
       </c>
@@ -808,27 +844,27 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>67</v>
       </c>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="H18">
         <v>67</v>
       </c>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>67</v>
       </c>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="G21">
         <v>96</v>
       </c>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B22">
         <v>67</v>
       </c>
@@ -836,7 +872,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
       <c r="J23">
         <v>96</v>
       </c>
@@ -847,16 +883,16 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="B3:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>0</v>
       </c>
@@ -864,7 +900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>0</v>
       </c>
@@ -872,12 +908,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="F8">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>0</v>
       </c>
@@ -891,7 +927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>36</v>
       </c>
@@ -899,7 +935,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C15">
         <v>0</v>
       </c>
@@ -910,21 +946,31 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:M13"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+  <dimension ref="C1:M18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="3" spans="3:13" x14ac:dyDescent="0.3">
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="I1">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="3" spans="3:13" x14ac:dyDescent="0.25">
       <c r="M3">
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="K4">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="5" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C5">
         <v>50</v>
       </c>
@@ -935,15 +981,135 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:13" x14ac:dyDescent="0.25">
       <c r="M7">
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="3:13" x14ac:dyDescent="0.25">
       <c r="G13">
         <v>50</v>
       </c>
+      <c r="M13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="I15">
+        <v>105</v>
+      </c>
+      <c r="J15">
+        <v>6</v>
+      </c>
+      <c r="K15">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="M17">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H18">
+        <v>3</v>
+      </c>
+      <c r="I18">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07D4DBED-60FF-4B30-BA86-F79481E892C2}">
+  <dimension ref="D3:G22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="E15" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D6">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <v>74</v>
+      </c>
+      <c r="F8">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="9" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E9">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="16" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D16">
+        <v>3</v>
+      </c>
+      <c r="E16">
+        <v>5</v>
+      </c>
+      <c r="F16">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F17">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F19">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="20" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F20">
+        <v>45</v>
+      </c>
+      <c r="G20">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="G21">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F22">
+        <v>4</v>
+      </c>
+      <c r="G22">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -951,21 +1117,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G1">
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>56</v>
       </c>
@@ -973,7 +1139,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D10">
         <v>38</v>
       </c>
@@ -984,16 +1150,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>31</v>
       </c>
@@ -1004,7 +1170,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J2">
         <v>28</v>
       </c>
@@ -1015,24 +1181,24 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F6">
         <v>38</v>
       </c>
@@ -1040,7 +1206,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D9">
         <v>29</v>
       </c>
@@ -1051,21 +1217,21 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B3:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>84</v>
       </c>
@@ -1073,12 +1239,12 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G6">
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D7">
         <v>22</v>
       </c>
@@ -1089,21 +1255,21 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="B2:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2">
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="G3">
         <v>87</v>
       </c>
@@ -1111,7 +1277,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C4">
         <v>0</v>
       </c>
@@ -1122,7 +1288,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="G5">
         <v>29</v>
       </c>
@@ -1130,7 +1296,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E6">
         <v>90</v>
       </c>
@@ -1138,7 +1304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>58</v>
       </c>
@@ -1149,16 +1315,16 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="B2:L10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.3">
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C2">
         <v>157</v>
       </c>
@@ -1169,12 +1335,12 @@
         <v>123</v>
       </c>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
       <c r="I3">
         <v>129</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C4">
         <v>62</v>
       </c>
@@ -1188,7 +1354,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="F6">
         <v>34</v>
       </c>
@@ -1199,7 +1365,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>157</v>
       </c>
@@ -1207,17 +1373,17 @@
         <v>858</v>
       </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D8">
         <v>94</v>
       </c>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="G9">
         <v>157</v>
       </c>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
       <c r="F10">
         <v>157</v>
       </c>
@@ -1228,16 +1394,16 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="B1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="2:8" x14ac:dyDescent="0.3">
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B1">
         <v>129</v>
       </c>
@@ -1248,7 +1414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C4">
         <v>100</v>
       </c>
@@ -1256,7 +1422,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>129</v>
       </c>
@@ -1264,17 +1430,17 @@
         <v>93</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D6">
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C8">
         <v>71</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>61</v>
       </c>
@@ -1291,16 +1457,16 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A2:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B2">
         <v>28</v>
       </c>
@@ -1320,7 +1486,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>0</v>
       </c>
@@ -1337,7 +1503,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>32</v>
       </c>
@@ -1363,7 +1529,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>56</v>
       </c>
@@ -1377,12 +1543,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E9">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>34</v>
       </c>

</xml_diff>